<commit_message>
Tracker update with iteration 4 pdf.
</commit_message>
<xml_diff>
--- a/Compliance Dashboard Progress Tracker.xlsx
+++ b/Compliance Dashboard Progress Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://northeastern-my.sharepoint.com/personal/toure_o_northeastern_edu/Documents/DS 5110/Final Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://northeastern-my.sharepoint.com/personal/toure_o_northeastern_edu/Documents/DS 5110/Final Project/Compliance-Detection-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E564CA0E-D068-4ED7-90C2-5EA30FE0E86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{E564CA0E-D068-4ED7-90C2-5EA30FE0E86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F81469DF-6070-4A38-97E9-40A52C849E9A}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{810C2B63-8FE3-4F75-8D7D-DD3680FE7D21}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="38700" windowHeight="15345" xr2:uid="{810C2B63-8FE3-4F75-8D7D-DD3680FE7D21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
   <si>
     <t>Phase</t>
   </si>
@@ -255,13 +255,16 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>Overall Progress (%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,8 +280,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,8 +331,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -498,11 +520,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -579,9 +632,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -913,20 +979,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0477E8-8128-4A84-A2F9-00B249EF2AA6}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
     <col min="4" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1" thickBot="1">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -942,8 +1008,12 @@
       <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1" thickBot="1">
       <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
@@ -959,8 +1029,13 @@
       <c r="E2" s="22" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="H2" s="28">
+        <f>ROUND( (COUNTIF(E2:E29,"Completed") + 0.5*COUNTIF(E2:E29,"In Progress")) / COUNTA(E2:E29) *100, 1)</f>
+        <v>53.6</v>
+      </c>
+      <c r="I2" s="29"/>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="45">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
@@ -977,7 +1052,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -991,10 +1066,10 @@
         <v>8</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
@@ -1008,10 +1083,10 @@
         <v>8</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -1025,10 +1100,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1042,10 +1117,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1">
       <c r="A8" s="9" t="s">
         <v>20</v>
       </c>
@@ -1059,10 +1134,10 @@
         <v>8</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
@@ -1076,10 +1151,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
@@ -1093,10 +1168,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -1110,10 +1185,10 @@
         <v>8</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -1127,10 +1202,10 @@
         <v>8</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1">
       <c r="A13" s="11" t="s">
         <v>31</v>
       </c>
@@ -1144,10 +1219,10 @@
         <v>8</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1">
       <c r="A14" s="11" t="s">
         <v>31</v>
       </c>
@@ -1161,10 +1236,10 @@
         <v>8</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="1" customFormat="1" ht="38.1" customHeight="1">
       <c r="A15" s="11" t="s">
         <v>31</v>
       </c>
@@ -1178,10 +1253,10 @@
         <v>8</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="38.1" customHeight="1">
       <c r="A16" s="11" t="s">
         <v>31</v>
       </c>
@@ -1195,10 +1270,10 @@
         <v>8</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="38.1" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>31</v>
       </c>
@@ -1212,10 +1287,10 @@
         <v>8</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="38.1" customHeight="1">
       <c r="A18" s="13" t="s">
         <v>42</v>
       </c>
@@ -1232,7 +1307,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="38.1" customHeight="1">
       <c r="A19" s="13" t="s">
         <v>42</v>
       </c>
@@ -1249,7 +1324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="38.1" customHeight="1">
       <c r="A20" s="13" t="s">
         <v>42</v>
       </c>
@@ -1266,7 +1341,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="38.1" customHeight="1">
       <c r="A21" s="13" t="s">
         <v>49</v>
       </c>
@@ -1283,7 +1358,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="38.1" customHeight="1">
       <c r="A22" s="13" t="s">
         <v>49</v>
       </c>
@@ -1300,7 +1375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="38.1" customHeight="1">
       <c r="A23" s="13" t="s">
         <v>49</v>
       </c>
@@ -1317,7 +1392,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="38.1" customHeight="1">
       <c r="A24" s="15" t="s">
         <v>56</v>
       </c>
@@ -1334,7 +1409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="38.1" customHeight="1">
       <c r="A25" s="15" t="s">
         <v>56</v>
       </c>
@@ -1351,7 +1426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="38.1" customHeight="1">
       <c r="A26" s="15" t="s">
         <v>56</v>
       </c>
@@ -1368,7 +1443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="38.1" customHeight="1">
       <c r="A27" s="15" t="s">
         <v>56</v>
       </c>
@@ -1385,7 +1460,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="38.1" customHeight="1">
       <c r="A28" s="15" t="s">
         <v>66</v>
       </c>
@@ -1402,7 +1477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="38.1" customHeight="1" thickBot="1">
       <c r="A29" s="17" t="s">
         <v>66</v>
       </c>
@@ -1421,6 +1496,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E29" xr:uid="{EF0477E8-8128-4A84-A2F9-00B249EF2AA6}"/>
+  <mergeCells count="2">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>